<commit_message>
done for 2 numbers
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,37 +424,191 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Hall Ticket No</t>
+          <t>HTNO</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Student Name</t>
+          <t>Edge Analytics</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Department</t>
+          <t>Cyber Security</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Marks Obtained</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Software Project Management</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Human Computer Interaction</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Renewable Energy Source</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Edge Analytics Lab</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Machine Learning Lab</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Internship / Mini Project</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>SGPA</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>CGPA</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Credits Obtained</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Subject Due</t>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>20J41A6901</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>790</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>9.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20J41A6902</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>746</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>8.58</t>
         </is>
       </c>
     </row>

</xml_diff>